<commit_message>
Add detail to report
</commit_message>
<xml_diff>
--- a/report/Data.xlsx
+++ b/report/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S2021\OpSysProject\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7907293B-3A73-4084-B7CA-3A65899450A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DBB83-1CDE-4652-8672-6F378A1988F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8889FC8-EFC9-4EC2-BD7A-6A18D966FDE7}"/>
+    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{E8889FC8-EFC9-4EC2-BD7A-6A18D966FDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>Run Number</t>
   </si>
@@ -87,7 +87,22 @@
     <t>I/O bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 4] [$\alpha$: 0.5] [$t_{slice}$: 2048] [rr_{add}: BEGINNING]}</t>
   </si>
   <si>
-    <t>I/O bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 20] [$\alpha$: 0.5] [$t_{slice}$: 2048]}</t>
+    <t>I/O bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 20] [$\alpha$: 0.5] [$t_{slice}$: 2048] [rr_{add}: BEGINNING]}</t>
+  </si>
+  <si>
+    <t>CPU bound {\tt [$n$: 1] [seed: 2] [$\lambda$: 0.01] [limit: 256] [$t_{cs}$: 4] [$\alpha$: 0.5] [$t_{slice}$: 128]}</t>
+  </si>
+  <si>
+    <t>CPU bound {\tt [$n$: 16] [seed: 2] [$\lambda$: 0.01] [limit: 256] [$t_{cs}$: 4] [$\alpha$: 0.75] [$t_{slice}$: 64]}</t>
+  </si>
+  <si>
+    <t>CPU bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 4] [$\alpha$: 0.5] [$t_{slice}$: 2048]}</t>
+  </si>
+  <si>
+    <t>CPU bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 4] [$\alpha$: 0.5] [$t_{slice}$: 2048][$rr_{add}$: BEGINNING]}</t>
+  </si>
+  <si>
+    <t>CPU bound {\tt [$n$: 8] [seed: 64] [$\lambda$: 0.001] [limit: 4096] [$t_{cs}$: 20] [$\alpha$: 0.5] [$t_{slice}$: 2048]}</t>
   </si>
 </sst>
 </file>
@@ -439,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC70030-D53F-4CBE-8EF7-E2AE4DC8471E}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,6 +1036,541 @@
         <v>38.305300000000003</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>1629.22</v>
+      </c>
+      <c r="D27">
+        <v>3216.87</v>
+      </c>
+      <c r="E27">
+        <v>4850.09</v>
+      </c>
+      <c r="F27">
+        <v>23</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>98.032600000000002</v>
+      </c>
+      <c r="I27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>1629.22</v>
+      </c>
+      <c r="D28">
+        <v>2596.35</v>
+      </c>
+      <c r="E28">
+        <v>4229.57</v>
+      </c>
+      <c r="F28">
+        <v>23</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>94.760300000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>1629.22</v>
+      </c>
+      <c r="D29">
+        <v>2543.5700000000002</v>
+      </c>
+      <c r="E29">
+        <v>4178.17</v>
+      </c>
+      <c r="F29">
+        <v>31</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>94.683599999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>1629.22</v>
+      </c>
+      <c r="D30">
+        <v>2249.39</v>
+      </c>
+      <c r="E30">
+        <v>3913.57</v>
+      </c>
+      <c r="F30">
+        <v>201</v>
+      </c>
+      <c r="G30">
+        <v>178</v>
+      </c>
+      <c r="H30">
+        <v>92.023600000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>1629.22</v>
+      </c>
+      <c r="D32">
+        <v>3216.87</v>
+      </c>
+      <c r="E32">
+        <v>4850.09</v>
+      </c>
+      <c r="F32">
+        <v>23</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>98.032600000000002</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>1629.22</v>
+      </c>
+      <c r="D33">
+        <v>2596.35</v>
+      </c>
+      <c r="E33">
+        <v>4229.57</v>
+      </c>
+      <c r="F33">
+        <v>23</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>94.760300000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>1629.22</v>
+      </c>
+      <c r="D34">
+        <v>2543.5700000000002</v>
+      </c>
+      <c r="E34">
+        <v>4178.17</v>
+      </c>
+      <c r="F34">
+        <v>31</v>
+      </c>
+      <c r="G34">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>94.683599999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>1629.22</v>
+      </c>
+      <c r="D35">
+        <v>2327.13</v>
+      </c>
+      <c r="E35">
+        <v>4024.17</v>
+      </c>
+      <c r="F35">
+        <v>390</v>
+      </c>
+      <c r="G35">
+        <v>367</v>
+      </c>
+      <c r="H35">
+        <v>90.068299999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>1629.22</v>
+      </c>
+      <c r="D37">
+        <v>3216.87</v>
+      </c>
+      <c r="E37">
+        <v>4850.09</v>
+      </c>
+      <c r="F37">
+        <v>23</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>98.032600000000002</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>1629.22</v>
+      </c>
+      <c r="D38">
+        <v>2730.65</v>
+      </c>
+      <c r="E38">
+        <v>4363.87</v>
+      </c>
+      <c r="F38">
+        <v>23</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>95.314599999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>1629.22</v>
+      </c>
+      <c r="D39">
+        <v>2017.39</v>
+      </c>
+      <c r="E39">
+        <v>3652.35</v>
+      </c>
+      <c r="F39">
+        <v>33</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>94.664500000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>1629.22</v>
+      </c>
+      <c r="D40">
+        <v>2829.35</v>
+      </c>
+      <c r="E40">
+        <v>4463.78</v>
+      </c>
+      <c r="F40">
+        <v>30</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>95.246799999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>1629.22</v>
+      </c>
+      <c r="D42">
+        <v>3216.87</v>
+      </c>
+      <c r="E42">
+        <v>4850.09</v>
+      </c>
+      <c r="F42">
+        <v>23</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>98.032600000000002</v>
+      </c>
+      <c r="I42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>1629.22</v>
+      </c>
+      <c r="D43">
+        <v>2730.65</v>
+      </c>
+      <c r="E43">
+        <v>4363.87</v>
+      </c>
+      <c r="F43">
+        <v>23</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>95.314599999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>1629.22</v>
+      </c>
+      <c r="D44">
+        <v>2017.39</v>
+      </c>
+      <c r="E44">
+        <v>3652.35</v>
+      </c>
+      <c r="F44">
+        <v>33</v>
+      </c>
+      <c r="G44">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>94.664500000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>1629.22</v>
+      </c>
+      <c r="D45">
+        <v>1743.61</v>
+      </c>
+      <c r="E45">
+        <v>3378.04</v>
+      </c>
+      <c r="F45">
+        <v>30</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45">
+        <v>95.616200000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>1629.22</v>
+      </c>
+      <c r="D47">
+        <v>3255.13</v>
+      </c>
+      <c r="E47">
+        <v>4904.3500000000004</v>
+      </c>
+      <c r="F47">
+        <v>23</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>97.097800000000007</v>
+      </c>
+      <c r="I47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>1629.22</v>
+      </c>
+      <c r="D48">
+        <v>2761.26</v>
+      </c>
+      <c r="E48">
+        <v>4410.4799999999996</v>
+      </c>
+      <c r="F48">
+        <v>23</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>94.430700000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>1629.22</v>
+      </c>
+      <c r="D49">
+        <v>2057.7399999999998</v>
+      </c>
+      <c r="E49">
+        <v>3715.65</v>
+      </c>
+      <c r="F49">
+        <v>33</v>
+      </c>
+      <c r="G49">
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <v>93.418400000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>1629.22</v>
+      </c>
+      <c r="D50">
+        <v>2876.65</v>
+      </c>
+      <c r="E50">
+        <v>4531.96</v>
+      </c>
+      <c r="F50">
+        <v>30</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
+        <v>94.098699999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
*.h => {*.hpp}, run formatter
</commit_message>
<xml_diff>
--- a/report/Data.xlsx
+++ b/report/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S2021\OpSysProject\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E44BFA-9AA5-4C8D-9316-17DB3AFD03C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231B1BA3-3D62-41AB-AE52-E93158396B36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8889FC8-EFC9-4EC2-BD7A-6A18D966FDE7}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,6 +1798,9 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>13</v>
+      </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
@@ -1824,6 +1827,9 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>13</v>
+      </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
@@ -1847,6 +1853,9 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>13</v>
+      </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
@@ -1869,7 +1878,10 @@
         <v>70.441299999999998</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>13</v>
+      </c>
       <c r="B65" t="s">
         <v>11</v>
       </c>
@@ -1892,7 +1904,10 @@
         <v>69.7958</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>14</v>
+      </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
@@ -1918,7 +1933,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>14</v>
+      </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
@@ -1941,7 +1959,10 @@
         <v>99.184200000000004</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>14</v>
+      </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
@@ -1964,7 +1985,10 @@
         <v>96.730999999999995</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>14</v>
+      </c>
       <c r="B70" t="s">
         <v>11</v>
       </c>

</xml_diff>